<commit_message>
updated video, bug report, and report. Added randomization
</commit_message>
<xml_diff>
--- a/PartA/Bug_Report.xlsx
+++ b/PartA/Bug_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwang\OneDrive\Desktop\MCGILL\FALL 2024\ECSE 429\Project\Part1\GitHub\ECSE429_Project_PartA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwang\OneDrive\Desktop\MCGILL\FALL 2024\ECSE 429\Project\Part1\GitHub\ECSE429_Project\PartA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A36259-1639-4246-A5FD-ACE4F34F6AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{986CE29B-A343-4F96-BCA1-F4130EAA2A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{19A62233-E936-4153-8FE9-C2F93DCC36CA}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>